<commit_message>
White box testing added tests
</commit_message>
<xml_diff>
--- a/WhiteBoxTesting.xlsx
+++ b/WhiteBoxTesting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SD6503_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D5500BC-9699-49AD-925B-F01164E6C146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE529A3D-0F2F-43D1-AD03-23247184B44B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{84DD0BDD-34A0-4121-B413-A041E4D23E14}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Test No.</t>
   </si>
@@ -53,106 +53,74 @@
     <t>Actual Result</t>
   </si>
   <si>
-    <t>btnSave_Click()                                     SaveStaffs()</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">Messagebox should display "Do you wish to Save the Staff Details?" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Messagebox displays "Do you wish to Save the Staff Details?" </t>
-  </si>
-  <si>
     <t>WHITE BOX TESTING</t>
   </si>
   <si>
-    <t>Form1.cs                            FileManager.cs</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Step 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Enter following text into textboxes:     Step 1(a) textbox Name:  "a"                                  Step 1(b) textbox ID:  "999999999999"                         Step 1(c) textbox DOB:  "a"                                      Step 1(d) txtbox Salary:  "999999999999"                     Step 1(e) textbox Email:  " a"                                  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Step 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Click on  Button "Save"</t>
-    </r>
-  </si>
-  <si>
     <t>Test Case</t>
   </si>
   <si>
-    <t>First name input only accepts string characters</t>
-  </si>
-  <si>
-    <t>First name text box accepts input</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user will not be able to save if the incorrect information is entered into the first name text box. </t>
-  </si>
-  <si>
-    <t>Emplyee.cs</t>
-  </si>
-  <si>
-    <t>Button Save Method</t>
-  </si>
-  <si>
-    <t>Enter the following to see the validation   :-            1234, !@#$, ????, &lt;blank&gt;, space, backspace, shift.</t>
-  </si>
-  <si>
-    <t>Entering non-string characters shows an error . Input box only accepts string data and control characters.</t>
-  </si>
-  <si>
     <t>Pass/Fail</t>
   </si>
   <si>
-    <t>TC_WBT_02</t>
-  </si>
-  <si>
-    <t>TC_WBT_01</t>
+    <t>Check Validation for “Location” field</t>
+  </si>
+  <si>
+    <t>TC_WHT_01</t>
+  </si>
+  <si>
+    <t>Match</t>
+  </si>
+  <si>
+    <t>Regular expression</t>
+  </si>
+  <si>
+    <t>Won’t create a match and an error message displayed saying “Only letters to be inputed”</t>
+  </si>
+  <si>
+    <t>Won’t create a match and an error message displayed saying letters to be inputed</t>
+  </si>
+  <si>
+    <t>Check Validation for “Date” field</t>
+  </si>
+  <si>
+    <t>TC_WHT_02</t>
+  </si>
+  <si>
+    <t>Won’t create a match and an error message displayed saying "Input Date in dd/mm/yyyy or dd-mm-yyyy format"</t>
+  </si>
+  <si>
+    <t>1. Enter “04-03/1999” into the date field.
+ 2. Press “Create” button</t>
+  </si>
+  <si>
+    <t>1. Enter “123” into the location field. 
+2. Press “Create” button</t>
+  </si>
+  <si>
+    <t>Authenticate Controller</t>
+  </si>
+  <si>
+    <t>LoginController</t>
+  </si>
+  <si>
+    <t>Authenticate</t>
+  </si>
+  <si>
+    <t>The app successfully authenticates the credentials with the ones in the cred.txt file</t>
+  </si>
+  <si>
+    <t>1. Enter “admin” into username input and password input .
+2. Press “Login” button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,13 +145,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -205,8 +166,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,8 +208,26 @@
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -243,60 +251,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="medium">
+        <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -304,35 +298,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -648,125 +639,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B856E9-6BC2-4688-8551-28BD4218AC9B}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="B1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" customWidth="1"/>
-    <col min="6" max="6" width="43.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" customWidth="1"/>
-    <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="C1" s="9" t="s">
+    <row r="1" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="C5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="F5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="H6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
-    </row>
-    <row r="32" spans="2:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="C32" s="9"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="10"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38" s="10"/>
+    </row>
+    <row r="19" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C20" s="4"/>
+    </row>
+    <row r="33" spans="4:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="3"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
WhiteBox testing added few tests
</commit_message>
<xml_diff>
--- a/WhiteBoxTesting.xlsx
+++ b/WhiteBoxTesting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SD6503_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE529A3D-0F2F-43D1-AD03-23247184B44B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C63127-EBC0-46C8-9108-EDC89B759D4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{84DD0BDD-34A0-4121-B413-A041E4D23E14}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Test No.</t>
   </si>
@@ -106,21 +106,41 @@
     <t>LoginController</t>
   </si>
   <si>
-    <t>Authenticate</t>
-  </si>
-  <si>
     <t>The app successfully authenticates the credentials with the ones in the cred.txt file</t>
   </si>
   <si>
     <t>1. Enter “admin” into username input and password input .
 2. Press “Login” button</t>
+  </si>
+  <si>
+    <t>Login/Index.cshtml
+LoginController.cs</t>
+  </si>
+  <si>
+    <t>Authenticate()</t>
+  </si>
+  <si>
+    <t>Login()</t>
+  </si>
+  <si>
+    <t>Login page functionality when Tab is pressed on Username field</t>
+  </si>
+  <si>
+    <t>1. Enter “admin” into username field.
+2. Press Tab button on keyboard</t>
+  </si>
+  <si>
+    <t>The cursor moves into password field</t>
+  </si>
+  <si>
+    <t>Login Page functionality for no username</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +211,12 @@
       <b/>
       <sz val="13"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -306,9 +332,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -323,6 +346,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -639,19 +665,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B856E9-6BC2-4688-8551-28BD4218AC9B}">
-  <dimension ref="B1:I39"/>
+  <dimension ref="B1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" customWidth="1"/>
     <col min="7" max="7" width="39.140625" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" customWidth="1"/>
@@ -659,137 +685,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="H4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="9" t="s">
+      <c r="E5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+    <row r="6" spans="2:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="2:9" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="9" t="s">
+    <row r="8" spans="2:9" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I8" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C20" s="4"/>
-    </row>
-    <row r="33" spans="4:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="D33" s="2"/>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="3"/>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="3"/>
+    <row r="21" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C22" s="4"/>
+    </row>
+    <row r="35" spans="4:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="3"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:G1"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated whitebox & testplan
</commit_message>
<xml_diff>
--- a/WhiteBoxTesting.xlsx
+++ b/WhiteBoxTesting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studying T2 2020\SD6503 Testing and Secure Coding\SD6503_Final_Project\Project\SD6503_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SD6503_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA0D92B-609D-4A78-A9A2-F25AE2D0D692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5C79AF-76EA-4F0B-8E0E-89BF33E4B3A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{84DD0BDD-34A0-4121-B413-A041E4D23E14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{84DD0BDD-34A0-4121-B413-A041E4D23E14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="119">
   <si>
     <t>Test No.</t>
   </si>
@@ -392,6 +392,21 @@
   </si>
   <si>
     <t>1. Enter “5” into the Saves field. 
+2. Press “Create” button</t>
+  </si>
+  <si>
+    <t>1. Enter "-1” into the Goals field. 
+2. Press “Create” button</t>
+  </si>
+  <si>
+    <t>Won’t create a statistics and an error message displayed saying “Please enter positive numbers”</t>
+  </si>
+  <si>
+    <t>1. Enter "-1” into the Assists field. 
+2. Press “Create” button</t>
+  </si>
+  <si>
+    <t>1. Enter "-1” into the Saves field. 
 2. Press “Create” button</t>
   </si>
 </sst>
@@ -908,26 +923,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B856E9-6BC2-4688-8551-28BD4218AC9B}">
-  <dimension ref="B1:I38"/>
+  <dimension ref="B1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="15.59765625" customWidth="1"/>
-    <col min="5" max="5" width="22.73046875" customWidth="1"/>
-    <col min="6" max="6" width="33.86328125" customWidth="1"/>
-    <col min="7" max="7" width="39.1328125" customWidth="1"/>
-    <col min="8" max="8" width="25.73046875" customWidth="1"/>
-    <col min="9" max="9" width="13.59765625" customWidth="1"/>
-    <col min="10" max="10" width="4.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="D1" s="8" t="s">
         <v>7</v>
       </c>
@@ -935,8 +950,8 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
@@ -962,7 +977,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>21</v>
       </c>
@@ -988,7 +1003,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:9" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>28</v>
       </c>
@@ -1014,7 +1029,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:9" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>31</v>
       </c>
@@ -1040,7 +1055,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>35</v>
       </c>
@@ -1066,7 +1081,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>85</v>
       </c>
@@ -1092,7 +1107,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:9" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>44</v>
       </c>
@@ -1118,7 +1133,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="89.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:9" ht="89.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
@@ -1144,7 +1159,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="89.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:9" ht="89.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
@@ -1170,7 +1185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="68.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:9" ht="68.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
@@ -1196,7 +1211,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>16</v>
       </c>
@@ -1222,7 +1237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>49</v>
       </c>
@@ -1248,7 +1263,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>49</v>
       </c>
@@ -1274,7 +1289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="68.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:9" ht="68.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>55</v>
       </c>
@@ -1300,7 +1315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:9" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>55</v>
       </c>
@@ -1326,7 +1341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="54.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:9" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>10</v>
       </c>
@@ -1352,7 +1367,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
@@ -1378,7 +1393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>55</v>
       </c>
@@ -1404,7 +1419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>55</v>
       </c>
@@ -1428,7 +1443,7 @@
       </c>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="69.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:9" ht="69.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>62</v>
       </c>
@@ -1454,7 +1469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="67.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:9" ht="67.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
         <v>62</v>
       </c>
@@ -1480,7 +1495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="68.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:9" ht="68.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
         <v>63</v>
       </c>
@@ -1506,7 +1521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="68.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:9" ht="68.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
         <v>63</v>
       </c>
@@ -1532,7 +1547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
         <v>75</v>
       </c>
@@ -1558,7 +1573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="70.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:9" ht="70.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
         <v>75</v>
       </c>
@@ -1584,12 +1599,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:9" ht="70.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>80</v>
@@ -1598,24 +1613,24 @@
         <v>13</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="68.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:9" ht="70.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>80</v>
@@ -1624,24 +1639,24 @@
         <v>13</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="67.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>80</v>
@@ -1650,24 +1665,24 @@
         <v>13</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:9" ht="68.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>80</v>
@@ -1676,7 +1691,7 @@
         <v>13</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>112</v>
@@ -1688,14 +1703,92 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="21" x14ac:dyDescent="0.65">
-      <c r="D32" s="1"/>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D35" s="2"/>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:9" ht="68.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="67.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="D35" s="1"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D38" s="2"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D41" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>